<commit_message>
Test + fichiers à zipper
</commit_message>
<xml_diff>
--- a/conception/Plan de test.xlsx
+++ b/conception/Plan de test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -47,7 +47,7 @@
     <t>Lucas</t>
   </si>
   <si>
-    <t>Premier test, sous Insomnia</t>
+    <t>Test manuel sous Insomnia</t>
   </si>
   <si>
     <t>Test récupération liste personnes API</t>
@@ -86,7 +86,7 @@
     <t>Échec</t>
   </si>
   <si>
-    <t>Première passe sur les tests automatiques</t>
+    <t>Test unitaire, sous JUnit5</t>
   </si>
   <si>
     <t>Test automatique getterAll API personne</t>
@@ -107,9 +107,6 @@
     <t>Périphérique sous format json</t>
   </si>
   <si>
-    <t>Test sous Insomnia</t>
-  </si>
-  <si>
     <t>Test récupération liste périphériques API</t>
   </si>
   <si>
@@ -125,13 +122,7 @@
     <t>Périphérique modifiée sous format json</t>
   </si>
   <si>
-    <t>Correction à la maison</t>
-  </si>
-  <si>
     <t>Test automatique getter API périphérique</t>
-  </si>
-  <si>
-    <t>Test fait à l'AFPA suite aux tests précédents de la veille</t>
   </si>
   <si>
     <t>Test automatique getterAll API périphérique</t>
@@ -155,13 +146,28 @@
     <t>Page index accédée</t>
   </si>
   <si>
-    <t>Premier test avec Selenium</t>
+    <t>Test d'intégration avec Selenium</t>
+  </si>
+  <si>
+    <t>Test automatique create API Ordinateur</t>
   </si>
   <si>
     <t>Fabien</t>
   </si>
   <si>
+    <t>Test automatique create API Smartphone</t>
+  </si>
+  <si>
     <t>Kenza</t>
+  </si>
+  <si>
+    <t>Test manuel sous Postman</t>
+  </si>
+  <si>
+    <t>Test récupération liste smartphone API</t>
+  </si>
+  <si>
+    <t>Test récupération smartphone API</t>
   </si>
 </sst>
 </file>
@@ -935,7 +941,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -943,7 +949,7 @@
         <v>45755.0</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>13</v>
@@ -958,7 +964,7 @@
         <v>10</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -966,7 +972,7 @@
         <v>45755.0</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>15</v>
@@ -981,7 +987,7 @@
         <v>10</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16">
@@ -989,7 +995,7 @@
         <v>45755.0</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>17</v>
@@ -1004,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -1012,13 +1018,13 @@
         <v>45755.0</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>9</v>
@@ -1027,7 +1033,7 @@
         <v>10</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
@@ -1050,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
@@ -1073,7 +1079,7 @@
         <v>10</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
@@ -1096,7 +1102,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
@@ -1119,7 +1125,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
@@ -1142,7 +1148,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
@@ -1150,7 +1156,7 @@
         <v>45757.0</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>21</v>
@@ -1165,7 +1171,7 @@
         <v>10</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
@@ -1173,7 +1179,7 @@
         <v>45757.0</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>21</v>
@@ -1188,7 +1194,7 @@
         <v>10</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
@@ -1196,7 +1202,7 @@
         <v>45757.0</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>21</v>
@@ -1211,7 +1217,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -1219,7 +1225,7 @@
         <v>45757.0</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>21</v>
@@ -1234,7 +1240,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
@@ -1242,7 +1248,7 @@
         <v>45757.0</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>21</v>
@@ -1257,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
@@ -1265,13 +1271,13 @@
         <v>45758.0</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>9</v>
@@ -1280,53 +1286,123 @@
         <v>10</v>
       </c>
       <c r="G28" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="10">
+        <v>45761.0</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10">
+        <v>45756.0</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
+      <c r="C30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
+      <c r="A31" s="10">
+        <v>40277.0</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
+      <c r="A32" s="10">
+        <v>45757.0</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="17"/>
+      <c r="A33" s="10">
+        <v>45758.0</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="14"/>
@@ -10128,7 +10204,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
@@ -10136,7 +10212,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">

</xml_diff>